<commit_message>
updated outputs-r202, previous copy of ful-path.csv
</commit_message>
<xml_diff>
--- a/outputs-HGR-r202/test-c__Coriobacteriia_split_pruned.xlsx
+++ b/outputs-HGR-r202/test-c__Coriobacteriia_split_pruned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>Row</t>
   </si>
@@ -274,7 +274,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -284,14 +284,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,638 +314,638 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>203.20167903122436</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1646.7305422674035</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>872.14354369114153</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>323.76553199081741</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>728.64048902913385</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2190.9670444342451</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>1410.0550192833773</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>1124.0207673191637</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+      <c r="A10" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>1266.1060628432158</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+      <c r="A11" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>1157.7559206782469</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
+      <c r="A12" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>1500.4264329474834</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
+      <c r="A13" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>1178.7976064932316</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
+      <c r="A14" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>386.71020757245412</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
+      <c r="A15" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>1581.7066342056148</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+      <c r="A16" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>1145.8722806278615</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
+      <c r="A17" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>837.93703421640862</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
+      <c r="A18" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>981.85540717133313</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
+      <c r="A19" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>1211.2726189184029</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
+      <c r="A20" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>668.45188820908834</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
+      <c r="A21" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>1013.2924982938403</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
+      <c r="A22" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>1212.7178150416805</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
+      <c r="A23" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>1350.1908329038092</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
+      <c r="A24" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2231.7205903852773</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
+      <c r="A25" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>1159.1638647738848</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
+      <c r="A26" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>1226.045907871752</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
+      <c r="A27" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>1350.3964681813904</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
+      <c r="A28" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>1364.7346240546942</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
+      <c r="A29" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>1689.2926672607064</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
+      <c r="A30" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>1255.4360945671133</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
+      <c r="A31" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>1991.609916884837</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
+      <c r="A32" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>1852.543489430527</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
+      <c r="A33" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2132.0151827861705</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
+      <c r="A34" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>1863.3657659711196</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
+      <c r="A35" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>552.23404321882299</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
+      <c r="A36" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>2164.8847371904217</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
+      <c r="A37" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>1664.7701446163917</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
+      <c r="A38" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>1632.3303167735785</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
+      <c r="A39" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>595.42095558256483</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
+      <c r="A40" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>1972.1063948975373</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
+      <c r="A41" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>1571.1983201577664</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
+      <c r="A42" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2151.8756578849366</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
+      <c r="A43" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>1252.394825567864</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
+      <c r="A44" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>1243.0688408568644</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
+      <c r="A45" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>1615.5555468411285</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
+      <c r="A46" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>1692.3729497236739</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
+      <c r="A47" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>1465.6206936305603</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
+      <c r="A48" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2107.1776440109365</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="s">
-        <v>48</v>
+      <c r="A49" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>981.6018919750411</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
+      <c r="A50" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>155.13848221849102</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>50</v>
+      <c r="A51" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>719.17032498576236</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="s">
-        <v>51</v>
+      <c r="A52" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>873.44690691267556</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
+      <c r="A53" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>1736.4951812591305</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
+      <c r="A54" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>1048.2976159585087</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="s">
-        <v>54</v>
+      <c r="A55" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>224.20213086907594</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
+      <c r="A56" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>241.12266500665604</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="s">
-        <v>56</v>
+      <c r="A57" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>870.16141821247857</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
-        <v>57</v>
+      <c r="A58" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>1228.1043312499246</v>
       </c>
       <c r="C58">
         <v>1</v>

</xml_diff>